<commit_message>
added map eval, and created Documentation Folder
</commit_message>
<xml_diff>
--- a/Deliverables/Code Review/Evaluation Results.xlsx
+++ b/Deliverables/Code Review/Evaluation Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\GitHub\Group-3-Repository\Deliverables\Code Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Batman\Desktop\Towson Spring 2021\COSC 412\Group_repo\Group-3-Repository\Deliverables\Code Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE6B786-860B-48E3-A0BB-72799782756C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCC64C4-9252-462C-B4C3-1F639EDFDDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
+    <workbookView xWindow="-22875" yWindow="90" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blog" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="67">
   <si>
     <t>Security in Word Press</t>
   </si>
@@ -194,6 +193,51 @@
   </si>
   <si>
     <t>Github repo or Description of change</t>
+  </si>
+  <si>
+    <t>Secure as the user input is handled by the plugin and the google api key is not accesable to the outside user .</t>
+  </si>
+  <si>
+    <t>Easy to maintan, more locations can be easily added, and as long as the number of hits to the page stay at a reasonable number there should be no charges for the API. The plugin can also be simply updated through the wp-admin page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure that the page is protected from bot spams or other attacks that could cause the API to be charged extra. </t>
+  </si>
+  <si>
+    <t>You can submit support requests through https://wpstorelocator.co/support/</t>
+  </si>
+  <si>
+    <t>Pretty simple setup, simply a plugin that manages location, and a google maps api key that provides the maps functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There Is doucmentation for how to manage the plugin and how it is connected to the google API https://wpstorelocator.co/documentation/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation on the how the Google Maps API key is set up, how billing is handled and what account it is on should all be created. </t>
+  </si>
+  <si>
+    <t>Tested the map from mulitple devices and locations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test the map on multiple browsers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map works quickly </t>
+  </si>
+  <si>
+    <t>The map functions correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a small annoyance, when you navigate to the page it asks your location and displays the gyms and parks near you, but to filter by gyms or parks you have to manually enter your location and search again. This will be worked on as a stretch Goal </t>
+  </si>
+  <si>
+    <t>Currently a few white boxes and a map make up the interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The interface could look a little better, maybe adding some round edges and making the filter options more clear. This will be worked on as a stretch Goal </t>
+  </si>
+  <si>
+    <t>Work well on the phone and desktop</t>
   </si>
 </sst>
 </file>
@@ -657,7 +701,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31681DCD-7B9F-4A8A-81F4-84F4BCA6FE0B}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1275,8 @@
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.7">
@@ -1263,62 +1308,106 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
@@ -1326,44 +1415,76 @@
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
@@ -1371,10 +1492,18 @@
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="11"/>
@@ -1390,7 +1519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A74BB3-BF8D-4A55-9D16-A52FBFD549DD}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added resolutions to Evaluation Results
</commit_message>
<xml_diff>
--- a/Deliverables/Code Review/Evaluation Results.xlsx
+++ b/Deliverables/Code Review/Evaluation Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Batman\Desktop\Towson Spring 2021\COSC 412\Group_repo\Group-3-Repository\Deliverables\Code Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F15F42E-B44F-4AD2-BB52-568FAC6265D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24B315D-5754-430E-8FFB-836D7B95D157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
   </bookViews>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="92">
   <si>
     <t>Security in Word Press</t>
   </si>
@@ -308,6 +307,12 @@
   </si>
   <si>
     <t>Work well on the phone and desktop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created Documentation file  for the Maps page: https://github.com/Hanandrof/Group-3-Repository/commit/49c4e95c0d54c951ddd50c763112b3d3e788061d#diff-c205924de0fe636ccdde4ed616fef66f75b78e98b03620637965c033fd161141 </t>
+  </si>
+  <si>
+    <t>Tested on Chrome, Firefox, Edge and Safari</t>
   </si>
 </sst>
 </file>
@@ -1442,7 +1447,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1455,8 @@
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.7">
@@ -1569,8 +1575,12 @@
       <c r="C9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="12">
+        <v>44312</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1582,8 +1592,12 @@
       <c r="C10" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="12">
+        <v>44312</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">

</xml_diff>

<commit_message>
added changes to eval results
</commit_message>
<xml_diff>
--- a/Deliverables/Code Review/Evaluation Results.xlsx
+++ b/Deliverables/Code Review/Evaluation Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\GitHub\Group-3-Repository\Deliverables\Code Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98354E7C-7F9C-4C68-BACD-E426EF1DFE50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8497F2B-CC9E-448B-A99D-1F11066FA3A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
   <si>
     <t>Security in Word Press</t>
   </si>
@@ -181,12 +181,6 @@
     <t>Wordpress Plugins Interactivity</t>
   </si>
   <si>
-    <t>Interaction between Buddy Press Groups and Buddy Press is not working. Groups is trying to give role permissions while Buddy Press is not accepting them.</t>
-  </si>
-  <si>
-    <t>Look into the documentation of Buddy Press and Buddy Press Groups and make sure they work together</t>
-  </si>
-  <si>
     <t>Make sure the plugins are working nice together. (Which they are not)</t>
   </si>
   <si>
@@ -194,6 +188,21 @@
   </si>
   <si>
     <t>Github repo or Description of change</t>
+  </si>
+  <si>
+    <t>Added simple documentation (must expand later)https://github.com/Hanandrof/Group-3-Repository/blob/main/Documentation/Blog_Documentation.pdf</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>Look into the documentation of Buddy Press and Paid Memberships Pro and make sure they work together</t>
+  </si>
+  <si>
+    <t>Interaction between Paid Memberships Pro and Buddy Press is not working. Groups is trying to give role permissions while Buddy Press is not accepting them.</t>
+  </si>
+  <si>
+    <t>I believe it has something to do with the multiple user plugins we had installed and it messed with the overall website</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -340,6 +349,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,7 +670,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,10 +701,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,7 +745,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -742,12 +755,14 @@
         <v>46</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -773,10 +788,12 @@
       <c r="C9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -786,8 +803,12 @@
       <c r="C10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="13">
+        <v>44313</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -921,10 +942,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1257,10 +1278,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1425,10 +1446,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
merged changes by Alex, Me (Jackson), Brandon, Akeem
</commit_message>
<xml_diff>
--- a/Deliverables/Code Review/Evaluation Results.xlsx
+++ b/Deliverables/Code Review/Evaluation Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\GitHub\Group-3-Repository\Deliverables\Code Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Batman\Desktop\Towson Spring 2021\COSC 412\Group_repo\Group-3-Repository\Deliverables\Code Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8497F2B-CC9E-448B-A99D-1F11066FA3A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37423C6D-07B7-48C2-BF5E-744DFBC823C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{31CC967A-23D1-4812-8F73-68A6D0814E2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blog" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="114">
   <si>
     <t>Security in Word Press</t>
   </si>
@@ -203,6 +203,183 @@
   </si>
   <si>
     <t>I believe it has something to do with the multiple user plugins we had installed and it messed with the overall website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loginizer Security protects the login from brute force attacks. </t>
+  </si>
+  <si>
+    <t>Users are allowed to use very weak passwords, it may be worth it to enforce stronger ones.</t>
+  </si>
+  <si>
+    <t>Added Paid Membership Pro - Require Strong Passwords plugin</t>
+  </si>
+  <si>
+    <t>High. Login is controlled primarily by Loginizer and Paid Membership Pro. Plugins are easy to maintain and there are only two.</t>
+  </si>
+  <si>
+    <t>Ensure that the plugins remain compatible and updated.</t>
+  </si>
+  <si>
+    <t>all plugins reviewed and disabled functions removed</t>
+  </si>
+  <si>
+    <t>The two plugins are working together without issue</t>
+  </si>
+  <si>
+    <t>Potentially add additional plugins for more functionality (password requirements)</t>
+  </si>
+  <si>
+    <t>See Security in Word Press above</t>
+  </si>
+  <si>
+    <t>Login takes two steps, select account type and then enter Username, Password, Email, Name</t>
+  </si>
+  <si>
+    <t>Documentation provided by plugins, including logs of login attacks and all user accounts and account details</t>
+  </si>
+  <si>
+    <t>Creation of different account levels with multiple usernames, including admin login</t>
+  </si>
+  <si>
+    <t>Account level assignment is half working, need to get BuddyPress to recognize the account levels.</t>
+  </si>
+  <si>
+    <t>Login is very quick, two easy steps</t>
+  </si>
+  <si>
+    <t>Namecheap auto backs up the site info</t>
+  </si>
+  <si>
+    <t>Check the backend of the site, contact namecheap support</t>
+  </si>
+  <si>
+    <t>role assignment can sometimes not get recognized by buddypress</t>
+  </si>
+  <si>
+    <t>update the buddypress plugin</t>
+  </si>
+  <si>
+    <t>BuddyPress and companion plugin were updated</t>
+  </si>
+  <si>
+    <t>servicable, looks like a login page, clear how to use</t>
+  </si>
+  <si>
+    <t>could write css to make more pretty, not high priority</t>
+  </si>
+  <si>
+    <t>Login page assesed by group and deemed perfectly servicable as is</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Ensure plugins are up-to-date, images potentially susceptible to hotlinking</t>
+  </si>
+  <si>
+    <t>Find a plugin to protect from Hotlinking</t>
+  </si>
+  <si>
+    <t>Easily maintained through plugin updates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep plugins current and ensure compatability </t>
+  </si>
+  <si>
+    <t>Primary format provided by Neve plugin</t>
+  </si>
+  <si>
+    <t>Neve compatability with other plugins</t>
+  </si>
+  <si>
+    <t>Visitor/Registered users can view pages based on user roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide further documentation </t>
+  </si>
+  <si>
+    <t>Able to view pages based on specified user role</t>
+  </si>
+  <si>
+    <t>Fair loading speed</t>
+  </si>
+  <si>
+    <t>Possibly resizing or compressing images</t>
+  </si>
+  <si>
+    <t>Namecheap provides automatic backups of site information.</t>
+  </si>
+  <si>
+    <t>contact namecheap support</t>
+  </si>
+  <si>
+    <t>Possible landing page if site were to go down</t>
+  </si>
+  <si>
+    <t>Prompt to join displayed for all users regardless of membership level</t>
+  </si>
+  <si>
+    <t>Display join now prompt to site visitors only</t>
+  </si>
+  <si>
+    <t>User friendly and welcoming to all</t>
+  </si>
+  <si>
+    <t>Keeping Design Consistent</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Secure as the user input is handled by the plugin and the google api key is not accesable to the outside user .</t>
+  </si>
+  <si>
+    <t>Easy to maintan, more locations can be easily added, and as long as the number of hits to the page stay at a reasonable number there should be no charges for the API. The plugin can also be simply updated through the wp-admin page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure that the page is protected from bot spams or other attacks that could cause the API to be charged extra. </t>
+  </si>
+  <si>
+    <t>You can submit support requests through https://wpstorelocator.co/support/</t>
+  </si>
+  <si>
+    <t>Pretty simple setup, simply a plugin that manages location, and a google maps api key that provides the maps functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There Is doucmentation for how to manage the plugin and how it is connected to the google API https://wpstorelocator.co/documentation/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation on the how the Google Maps API key is set up, how billing is handled and what account it is on should all be created. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created Documentation file  for the Maps page: https://github.com/Hanandrof/Group-3-Repository/commit/49c4e95c0d54c951ddd50c763112b3d3e788061d#diff-c205924de0fe636ccdde4ed616fef66f75b78e98b03620637965c033fd161141 </t>
+  </si>
+  <si>
+    <t>Tested the map from mulitple devices and locations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test the map on multiple browsers </t>
+  </si>
+  <si>
+    <t>Tested on Chrome, Firefox, Edge and Safari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map works quickly </t>
+  </si>
+  <si>
+    <t>The map functions correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a small annoyance, when you navigate to the page it asks your location and displays the gyms and parks near you, but to filter by gyms or parks you have to manually enter your location and search again. This will be worked on as a stretch Goal </t>
+  </si>
+  <si>
+    <t>Currently a few white boxes and a map make up the interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The interface could look a little better, maybe adding some round edges and making the filter options more clear. This will be worked on as a stretch Goal </t>
+  </si>
+  <si>
+    <t>Work well on the phone and desktop</t>
   </si>
 </sst>
 </file>
@@ -318,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -353,6 +530,80 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C93C76-FF1F-4748-96EE-1115D9605DB1}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -912,7 +1163,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,154 +1171,258 @@
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>23</v>
       </c>
+      <c r="E1" s="14"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="24">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="24">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="24">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="B11" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B12" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="24">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="24">
+        <v>44312</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1080,7 +1435,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E17"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,154 +1443,210 @@
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
         <v>24</v>
       </c>
+      <c r="E1" s="25"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="33" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="B8" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="B14" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1247,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31681DCD-7B9F-4A8A-81F4-84F4BCA6FE0B}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,154 +1667,250 @@
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35" t="s">
         <v>21</v>
       </c>
+      <c r="E1" s="35"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="45" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B5" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="44">
+        <v>44312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="44">
+        <v>44312</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B11" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="B12" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B14" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="B15" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed adding information to Evaluation.xlsx
</commit_message>
<xml_diff>
--- a/Deliverables/Code Review/Evaluation Results.xlsx
+++ b/Deliverables/Code Review/Evaluation Results.xlsx
@@ -562,7 +562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -623,10 +623,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,7 +646,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>
@@ -900,7 +896,7 @@
       <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>
@@ -1177,7 +1173,7 @@
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>
@@ -1406,12 +1402,12 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.42"/>
   </cols>
   <sheetData>
@@ -1433,10 +1429,10 @@
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1672,10 +1668,10 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.71"/>

</xml_diff>